<commit_message>
Trying to get the shifting more consistent
</commit_message>
<xml_diff>
--- a/Observations/2022-02-19/14in/Targets/NGC2346/Shifts/ha/2022-02-19_NGC2346_ha_shifts.xlsx
+++ b/Observations/2022-02-19/14in/Targets/NGC2346/Shifts/ha/2022-02-19_NGC2346_ha_shifts.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -46,11 +46,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -62,6 +63,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -74,8 +76,8 @@
   <dimension ref="A1:B16"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1875" customWidth="true"/>
-    <col min="2" max="2" width="12.1875" customWidth="true"/>
+    <col min="1" max="1" width="12.42578125" customWidth="true"/>
+    <col min="2" max="2" width="12.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>